<commit_message>
adding work from the past week. bug fixes and finishing data crunching pipeline.
</commit_message>
<xml_diff>
--- a/data/Hotel_Names_Addresses_Distances.xlsx
+++ b/data/Hotel_Names_Addresses_Distances.xlsx
@@ -1217,7 +1217,7 @@
   <dimension ref="A1:G179"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3287,16 +3287,16 @@
         <v>183</v>
       </c>
       <c r="D90" s="0" t="n">
-        <v>1.05846755245086</v>
+        <v>1.05274359240546</v>
       </c>
       <c r="E90" s="0" t="n">
-        <v>2.26407927833353</v>
+        <v>2.25860503435984</v>
       </c>
       <c r="F90" s="0" t="n">
-        <v>0.404540162914151</v>
+        <v>0.404405959899717</v>
       </c>
       <c r="G90" s="0" t="n">
-        <v>3.06289339854317</v>
+        <v>3.06751543684017</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>